<commit_message>
Update TPS Pillar and SubPillar names
</commit_message>
<xml_diff>
--- a/CD-valid/Outcomes/Pretest/Czechia/Czechia.xlsx
+++ b/CD-valid/Outcomes/Pretest/Czechia/Czechia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -250,6 +250,12 @@
     <t xml:space="preserve">yellow</t>
   </si>
   <si>
+    <t xml:space="preserve">1: Constraints on Government Powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.02: Judicial Constraints</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL_courtrulings_imp</t>
   </si>
   <si>
@@ -265,7 +271,7 @@
     <t xml:space="preserve">SPE_534_QA15_7</t>
   </si>
   <si>
-    <t xml:space="preserve">1.03</t>
+    <t xml:space="preserve">1.03: Independent Oversight</t>
   </si>
   <si>
     <t xml:space="preserve">ORC_impartial_measures</t>
@@ -277,6 +283,12 @@
     <t xml:space="preserve">green</t>
   </si>
   <si>
+    <t xml:space="preserve">1.04: Elections are free, fair, and secure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.05: Non-governmental checks</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freedom in the World</t>
   </si>
   <si>
@@ -289,7 +301,7 @@
     <t xml:space="preserve">Varieties of Democracy</t>
   </si>
   <si>
-    <t xml:space="preserve">1.06</t>
+    <t xml:space="preserve">1.06: Respect for the legitimacy of the constitutional order, the law making process, and political opponents (absence of authoritarianism)</t>
   </si>
   <si>
     <t xml:space="preserve">PAB_overcourts</t>
@@ -298,7 +310,7 @@
     <t xml:space="preserve">VDM_v2juhccomp</t>
   </si>
   <si>
-    <t xml:space="preserve">1.07</t>
+    <t xml:space="preserve">1.07: Respect for judicial independence (absence of authoritarianism)</t>
   </si>
   <si>
     <t xml:space="preserve">PAB_manipulelect</t>
@@ -307,7 +319,7 @@
     <t xml:space="preserve">SPE_507_qb1_2</t>
   </si>
   <si>
-    <t xml:space="preserve">1.09</t>
+    <t xml:space="preserve">1.09: Respect for the electoral process (absence of authoritarianism)</t>
   </si>
   <si>
     <t xml:space="preserve">PAB_attackmedia</t>
@@ -316,7 +328,7 @@
     <t xml:space="preserve">VDM_v2csreprss</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1</t>
+    <t xml:space="preserve">1.1: Respect for civil liberties (absence of authoritarianism)</t>
   </si>
   <si>
     <t xml:space="preserve">PAB_misinfo</t>
@@ -331,7 +343,7 @@
     <t xml:space="preserve">SPE_489_qa4_5</t>
   </si>
   <si>
-    <t xml:space="preserve">1.11</t>
+    <t xml:space="preserve">1.11: Government officials who abuse their power are sanctioned for misconduct (accountability and sanctions for misconduct)</t>
   </si>
   <si>
     <t xml:space="preserve">LEP_bribesreq</t>
@@ -343,7 +355,7 @@
     <t xml:space="preserve">Global Corruption Barometer</t>
   </si>
   <si>
-    <t xml:space="preserve">1.12</t>
+    <t xml:space="preserve">1.12: Government officials who commit crimes are prosecuted and punished (accountability and sanctions for misconduct)</t>
   </si>
   <si>
     <t xml:space="preserve">ORC_corimpact</t>
@@ -352,6 +364,12 @@
     <t xml:space="preserve">SPE_534_QA15_4</t>
   </si>
   <si>
+    <t xml:space="preserve">2: Absence of Corruption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1: Absence of Bribery</t>
+  </si>
+  <si>
     <t xml:space="preserve">COR_3year_change</t>
   </si>
   <si>
@@ -364,7 +382,7 @@
     <t xml:space="preserve">SPE_489_qa4_4</t>
   </si>
   <si>
-    <t xml:space="preserve">2.4</t>
+    <t xml:space="preserve">2.4: Absence of nepotism, favoritism, and patronage</t>
   </si>
   <si>
     <t xml:space="preserve">ORC_pconnections</t>
@@ -379,7 +397,10 @@
     <t xml:space="preserve">SPE_534_QA15_10</t>
   </si>
   <si>
-    <t xml:space="preserve">3.1</t>
+    <t xml:space="preserve">3: Open Government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1: Right to information is effectively guaranteed</t>
   </si>
   <si>
     <t xml:space="preserve">IPR_easy2read</t>
@@ -409,6 +430,9 @@
     <t xml:space="preserve">FRS_Views on authorities making information easy to find without using the internet</t>
   </si>
   <si>
+    <t xml:space="preserve">3.2: Civic participation is effectively guaranteed</t>
+  </si>
+  <si>
     <t xml:space="preserve">CPA_protest</t>
   </si>
   <si>
@@ -430,13 +454,19 @@
     <t xml:space="preserve">ESS_trstprl</t>
   </si>
   <si>
+    <t xml:space="preserve">4: Fundamental Rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.2: Freedoms</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL_equality_imp</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_489_qa2_1</t>
   </si>
   <si>
-    <t xml:space="preserve">4.3</t>
+    <t xml:space="preserve">4.3: Equality</t>
   </si>
   <si>
     <t xml:space="preserve">CTZ_laborcond_A</t>
@@ -445,18 +475,24 @@
     <t xml:space="preserve">EWC_osh_risk</t>
   </si>
   <si>
-    <t xml:space="preserve">4.4</t>
+    <t xml:space="preserve">4.4: Solidarity</t>
   </si>
   <si>
     <t xml:space="preserve">EWC_work_life_balance</t>
   </si>
   <si>
+    <t xml:space="preserve">4.5: Citizens' Rights</t>
+  </si>
+  <si>
     <t xml:space="preserve">JSE_equality</t>
   </si>
   <si>
     <t xml:space="preserve">ESS_cttresac</t>
   </si>
   <si>
+    <t xml:space="preserve">4.6: Justice</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL_constprotection_imp</t>
   </si>
   <si>
@@ -472,16 +508,19 @@
     <t xml:space="preserve">Organized Crime Index</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.2</t>
+    <t xml:space="preserve">5: Order and Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.2: Absence of crime and violence</t>
   </si>
   <si>
     <t xml:space="preserve">JSE_rightsaware</t>
   </si>
   <si>
-    <t xml:space="preserve">7.1</t>
+    <t xml:space="preserve">7: Civil Justice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.1: Legal security</t>
   </si>
   <si>
     <t xml:space="preserve">JSE_access2assis</t>
@@ -490,7 +529,7 @@
     <t xml:space="preserve">VDM_v2clacjstm</t>
   </si>
   <si>
-    <t xml:space="preserve">7.2</t>
+    <t xml:space="preserve">7.2: People can access quality legal assistance and representation</t>
   </si>
   <si>
     <t xml:space="preserve">VDM_v2clacjstw</t>
@@ -502,19 +541,34 @@
     <t xml:space="preserve">SPE_489_qa5_2</t>
   </si>
   <si>
-    <t xml:space="preserve">7.3</t>
+    <t xml:space="preserve">7.3: Civil justice is people-centered, accessible, efficient, and outcome-oriented</t>
   </si>
   <si>
     <t xml:space="preserve">JSE_quickresol</t>
   </si>
   <si>
+    <t xml:space="preserve">7.4: Civil justice is impartial and free from corruption and undue influence</t>
+  </si>
+  <si>
     <t xml:space="preserve">JSE_enforce</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_489_qa6_1</t>
   </si>
   <si>
-    <t xml:space="preserve">7.5</t>
+    <t xml:space="preserve">7.5: Civil justice is effectively enforced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: Criminal Justice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.1: Criminal Investigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.2: Prosecution and pre-trial process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.3: Adjudication</t>
   </si>
   <si>
     <t xml:space="preserve">CJP_resprights</t>
@@ -523,7 +577,10 @@
     <t xml:space="preserve">FRS_Perception of the way the police generally treats people</t>
   </si>
   <si>
-    <t xml:space="preserve">8.5</t>
+    <t xml:space="preserve">8.5: Victim's Rights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.6: Due process of law</t>
   </si>
   <si>
     <t xml:space="preserve">CJP_saferights</t>
@@ -532,7 +589,7 @@
     <t xml:space="preserve">VDM_v2cltort</t>
   </si>
   <si>
-    <t xml:space="preserve">8.7</t>
+    <t xml:space="preserve">8.7: Prisons</t>
   </si>
   <si>
     <t xml:space="preserve">country_code</t>
@@ -998,7 +1055,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000218550210143476</v>
+        <v>0.000218550210143478</v>
       </c>
       <c r="D4" t="n">
         <v>0.514492753623188</v>
@@ -1085,7 +1142,7 @@
         <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00556601791449784</v>
+        <v>0.00556601791449782</v>
       </c>
       <c r="D7" t="n">
         <v>0.439024390243902</v>
@@ -1143,7 +1200,7 @@
         <v>30</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0000000023018649613526</v>
+        <v>0.00000000230186496135259</v>
       </c>
       <c r="D9" t="n">
         <v>0.8125</v>
@@ -1178,7 +1235,7 @@
         <v>0.625</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0519399249061326</v>
+        <v>0.0519399249061327</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -1230,7 +1287,7 @@
         <v>40</v>
       </c>
       <c r="C12" t="n">
-        <v>0.00000396811402841639</v>
+        <v>0.00000396811402841638</v>
       </c>
       <c r="D12" t="n">
         <v>0.395833333333333</v>
@@ -1346,7 +1403,7 @@
         <v>25</v>
       </c>
       <c r="C16" t="n">
-        <v>0.00556601791449784</v>
+        <v>0.00556601791449782</v>
       </c>
       <c r="D16" t="n">
         <v>0.439024390243902</v>
@@ -1404,7 +1461,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="n">
-        <v>0.000218550210143476</v>
+        <v>0.000218550210143478</v>
       </c>
       <c r="D18" t="n">
         <v>0.514492753623188</v>
@@ -1491,7 +1548,7 @@
         <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>0.00556601791449784</v>
+        <v>0.00556601791449782</v>
       </c>
       <c r="D21" t="n">
         <v>0.439024390243902</v>
@@ -1520,7 +1577,7 @@
         <v>45</v>
       </c>
       <c r="C22" t="n">
-        <v>0.375236954069154</v>
+        <v>0.375236954069153</v>
       </c>
       <c r="D22" t="n">
         <v>0.515151515151515</v>
@@ -1549,7 +1606,7 @@
         <v>48</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0015495925712325</v>
+        <v>0.00154959257123249</v>
       </c>
       <c r="D23" t="n">
         <v>0.481060606060606</v>
@@ -1607,7 +1664,7 @@
         <v>48</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0015495925712325</v>
+        <v>0.00154959257123249</v>
       </c>
       <c r="D25" t="n">
         <v>0.481060606060606</v>
@@ -1694,7 +1751,7 @@
         <v>60</v>
       </c>
       <c r="C28" t="n">
-        <v>0.727936265627073</v>
+        <v>0.727936265627074</v>
       </c>
       <c r="D28" t="n">
         <v>0.423611111111111</v>
@@ -1723,10 +1780,10 @@
         <v>62</v>
       </c>
       <c r="C29" t="n">
-        <v>0.074606609890559</v>
+        <v>0.0746066098905587</v>
       </c>
       <c r="D29" t="n">
-        <v>0.537414965986394</v>
+        <v>0.537414965986395</v>
       </c>
       <c r="E29" t="n">
         <v>0.431457431457431</v>
@@ -1845,10 +1902,10 @@
         <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
@@ -1856,13 +1913,13 @@
         <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" t="n">
         <v>0.569444444444444</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E3" t="n">
         <v>0.260980592441267</v>
@@ -1874,13 +1931,13 @@
         <v>0.308463852003178</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
@@ -1888,13 +1945,13 @@
         <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" t="n">
         <v>0.479674796747967</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E4" t="n">
         <v>0.679902473005921</v>
@@ -1909,10 +1966,10 @@
         <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
@@ -1920,13 +1977,13 @@
         <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C5" t="n">
         <v>0.527131782945736</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E5" t="n">
         <v>0.608050019538882</v>
@@ -1938,13 +1995,13 @@
         <v>0.080918236593146</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
@@ -1973,10 +2030,10 @@
         <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
@@ -2002,13 +2059,13 @@
         <v>0.0884283969998255</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -2037,10 +2094,10 @@
         <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
@@ -2066,13 +2123,13 @@
         <v>0.0252494165320202</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
@@ -2092,19 +2149,19 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G10" t="n">
         <v>0.425</v>
       </c>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -2124,19 +2181,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G11" t="n">
         <v>0.495495495495496</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
@@ -2144,31 +2201,31 @@
         <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C12" t="n">
         <v>0.577777777777778</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E12" t="n">
         <v>0.483167782183002</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G12" t="n">
         <v>0.0946099955947761</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13">
@@ -2176,31 +2233,31 @@
         <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C13" t="n">
         <v>0.5</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E13" t="n">
         <v>0.509136975455265</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G13" t="n">
         <v>0.00913697545526526</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14">
@@ -2208,13 +2265,13 @@
         <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C14" t="n">
         <v>0.558823529411765</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E14" t="n">
         <v>0.28757546870035</v>
@@ -2226,13 +2283,13 @@
         <v>0.271248060711415</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J14" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15">
@@ -2240,31 +2297,31 @@
         <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C15" t="n">
         <v>0.530612244897959</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E15" t="n">
         <v>0.611451306841004</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G15" t="n">
         <v>0.0808390619430452</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16">
@@ -2272,13 +2329,13 @@
         <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C16" t="n">
         <v>0.412698412698413</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E16" t="n">
         <v>0.22952380952381</v>
@@ -2293,10 +2350,10 @@
         <v>77</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17">
@@ -2304,13 +2361,13 @@
         <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C17" t="n">
         <v>0.487341772151899</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E17" t="n">
         <v>0.131155778894472</v>
@@ -2322,13 +2379,13 @@
         <v>0.356185993257426</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J17" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18">
@@ -2336,31 +2393,31 @@
         <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C18" t="n">
         <v>0.517543859649123</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E18" t="n">
         <v>0.422395273899033</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G18" t="n">
         <v>0.0951485857500894</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19">
@@ -2368,13 +2425,13 @@
         <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C19" t="n">
         <v>0.514767932489451</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E19" t="n">
         <v>0.755873340143003</v>
@@ -2389,10 +2446,10 @@
         <v>77</v>
       </c>
       <c r="I19" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="J19" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20">
@@ -2400,13 +2457,13 @@
         <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C20" t="n">
         <v>0.478658536585366</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E20" t="n">
         <v>0.391025641025641</v>
@@ -2415,16 +2472,16 @@
         <v>76</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0876328955597249</v>
+        <v>0.0876328955597248</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="J20" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21">
@@ -2450,13 +2507,13 @@
         <v>0.699004975124378</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I21" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="J21" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22">
@@ -2476,19 +2533,19 @@
         <v>0.0218446601941748</v>
       </c>
       <c r="F22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G22" t="n">
         <v>0.603155339805825</v>
       </c>
       <c r="H22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="J22" t="s">
-        <v>32</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23">
@@ -2496,13 +2553,13 @@
         <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C23" t="n">
         <v>0.449367088607595</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E23" t="n">
         <v>0.175200803212851</v>
@@ -2514,13 +2571,13 @@
         <v>0.274166285394744</v>
       </c>
       <c r="H23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="J23" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24">
@@ -2528,13 +2585,13 @@
         <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C24" t="n">
         <v>0.57088122605364</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E24" t="n">
         <v>0.52060737527115</v>
@@ -2546,13 +2603,13 @@
         <v>0.0502738507824901</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I24" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="J24" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
@@ -2560,13 +2617,13 @@
         <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C25" t="n">
         <v>0.488636363636364</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E25" t="n">
         <v>0.643249176728869</v>
@@ -2581,10 +2638,10 @@
         <v>77</v>
       </c>
       <c r="I25" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J25" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26">
@@ -2592,19 +2649,19 @@
         <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C26" t="n">
         <v>0.542635658914729</v>
       </c>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E26" t="n">
         <v>0.752525252525253</v>
       </c>
       <c r="F26" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G26" t="n">
         <v>0.209889593610524</v>
@@ -2613,10 +2670,10 @@
         <v>77</v>
       </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J26" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27">
@@ -2624,19 +2681,19 @@
         <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C27" t="n">
         <v>0.546511627906977</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E27" t="n">
         <v>0.686868686868687</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G27" t="n">
         <v>0.14035705896171</v>
@@ -2645,10 +2702,10 @@
         <v>77</v>
       </c>
       <c r="I27" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J27" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28">
@@ -2656,31 +2713,31 @@
         <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="C28" t="n">
         <v>0.491452991452991</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E28" t="n">
         <v>0.752577319587629</v>
       </c>
       <c r="F28" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G28" t="n">
         <v>0.261124328134637</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J28" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
@@ -2688,31 +2745,31 @@
         <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C29" t="n">
         <v>0.524390243902439</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E29" t="n">
         <v>0.622448979591837</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G29" t="n">
         <v>0.0980587356893977</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I29" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J29" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30">
@@ -2741,10 +2798,10 @@
         <v>77</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J30" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31">
@@ -2770,13 +2827,13 @@
         <v>0.0252494165320202</v>
       </c>
       <c r="H31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I31" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J31" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32">
@@ -2796,19 +2853,19 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G32" t="n">
         <v>0.425</v>
       </c>
       <c r="H32" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I32" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33">
@@ -2828,19 +2885,19 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G33" t="n">
         <v>0.495495495495496</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I33" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J33" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34">
@@ -2848,31 +2905,31 @@
         <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C34" t="n">
         <v>0.5</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E34" t="n">
         <v>0.0628803245436105</v>
       </c>
       <c r="F34" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G34" t="n">
         <v>0.437119675456389</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I34" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J34" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35">
@@ -2880,31 +2937,31 @@
         <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C35" t="n">
         <v>0.419354838709677</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E35" t="n">
         <v>0.0568412505075112</v>
       </c>
       <c r="F35" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G35" t="n">
         <v>0.362513588202166</v>
       </c>
       <c r="H35" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I35" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J35" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36">
@@ -2912,31 +2969,31 @@
         <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C36" t="n">
         <v>0.478927203065134</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E36" t="n">
         <v>0.468680182043856</v>
       </c>
       <c r="F36" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G36" t="n">
         <v>0.0102470210212781</v>
       </c>
       <c r="H36" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I36" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J36" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37">
@@ -2956,7 +3013,7 @@
         <v>0.644869706840391</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G37" t="n">
         <v>0.126351188321872</v>
@@ -2965,10 +3022,10 @@
         <v>77</v>
       </c>
       <c r="I37" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J37" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38">
@@ -2988,19 +3045,19 @@
         <v>0.383012689316414</v>
       </c>
       <c r="F38" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G38" t="n">
         <v>0.0128206440169191</v>
       </c>
       <c r="H38" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I38" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="J38" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39">
@@ -3029,10 +3086,10 @@
         <v>77</v>
       </c>
       <c r="I39" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J39" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40">
@@ -3058,13 +3115,13 @@
         <v>0.0252494165320202</v>
       </c>
       <c r="H40" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I40" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J40" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41">
@@ -3084,19 +3141,19 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G41" t="n">
         <v>0.425</v>
       </c>
       <c r="H41" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I41" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J41" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42">
@@ -3116,19 +3173,19 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G42" t="n">
         <v>0.495495495495496</v>
       </c>
       <c r="H42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I42" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J42" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43">
@@ -3136,13 +3193,13 @@
         <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C43" t="n">
-        <v>0.52906976744186</v>
+        <v>0.529069767441861</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E43" t="n">
         <v>0.196446700507614</v>
@@ -3154,13 +3211,13 @@
         <v>0.332623066934246</v>
       </c>
       <c r="H43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I43" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J43" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44">
@@ -3168,13 +3225,13 @@
         <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C44" t="n">
         <v>0.591666666666667</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E44" t="n">
         <v>0.752525252525252</v>
@@ -3189,10 +3246,10 @@
         <v>77</v>
       </c>
       <c r="I44" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J44" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45">
@@ -3200,13 +3257,13 @@
         <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C45" t="n">
         <v>0.591666666666667</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="E45" t="n">
         <v>0.688676075268817</v>
@@ -3218,13 +3275,13 @@
         <v>0.0970094086021505</v>
       </c>
       <c r="H45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I45" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J45" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46">
@@ -3253,10 +3310,10 @@
         <v>77</v>
       </c>
       <c r="I46" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J46" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47">
@@ -3264,19 +3321,19 @@
         <v>75</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C47" t="n">
         <v>0.418439716312057</v>
       </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E47" t="n">
         <v>0.53935860058309</v>
       </c>
       <c r="F47" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G47" t="n">
         <v>0.120918884271034</v>
@@ -3285,10 +3342,10 @@
         <v>77</v>
       </c>
       <c r="I47" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J47" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48">
@@ -3296,13 +3353,13 @@
         <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C48" t="n">
         <v>0.486842105263158</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="E48" t="n">
         <v>0.763299663299663</v>
@@ -3314,13 +3371,13 @@
         <v>0.276457558036505</v>
       </c>
       <c r="H48" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I48" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J48" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49">
@@ -3340,19 +3397,19 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G49" t="n">
         <v>0.484848484848485</v>
       </c>
       <c r="H49" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I49" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="J49" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50">
@@ -3360,19 +3417,19 @@
         <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C50" t="n">
         <v>0.431034482758621</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="E50" t="n">
         <v>0.591111111111111</v>
       </c>
       <c r="F50" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="G50" t="n">
         <v>0.16007662835249</v>
@@ -3381,10 +3438,10 @@
         <v>77</v>
       </c>
       <c r="I50" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="J50" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51">
@@ -3392,31 +3449,31 @@
         <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C51" t="n">
         <v>0.446808510638298</v>
       </c>
       <c r="D51" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E51" t="n">
         <v>0.752525252525253</v>
       </c>
       <c r="F51" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G51" t="n">
         <v>0.305716741886955</v>
       </c>
       <c r="H51" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I51" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J51" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52">
@@ -3424,31 +3481,31 @@
         <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C52" t="n">
         <v>0.503875968992248</v>
       </c>
       <c r="D52" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="E52" t="n">
         <v>0.548034598454766</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G52" t="n">
         <v>0.0441586294625184</v>
       </c>
       <c r="H52" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I52" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J52" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53">
@@ -3456,31 +3513,31 @@
         <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C53" t="n">
         <v>0.503875968992248</v>
       </c>
       <c r="D53" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="E53" t="n">
         <v>0.497777444253569</v>
       </c>
       <c r="F53" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G53" t="n">
         <v>0.00609852473867861</v>
       </c>
       <c r="H53" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I53" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J53" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54">
@@ -3488,13 +3545,13 @@
         <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="C54" t="n">
         <v>0.486111111111111</v>
       </c>
       <c r="D54" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="E54" t="n">
         <v>0.772018970189702</v>
@@ -3506,13 +3563,13 @@
         <v>0.285907859078591</v>
       </c>
       <c r="H54" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I54" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J54" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55">
@@ -3520,13 +3577,13 @@
         <v>75</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C55" t="n">
         <v>0.526666666666667</v>
       </c>
       <c r="D55" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="E55" t="n">
         <v>0.772018970189702</v>
@@ -3541,10 +3598,10 @@
         <v>77</v>
       </c>
       <c r="I55" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J55" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56">
@@ -3573,10 +3630,10 @@
         <v>77</v>
       </c>
       <c r="I56" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J56" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57">
@@ -3596,7 +3653,7 @@
         <v>0.679487179487179</v>
       </c>
       <c r="F57" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G57" t="n">
         <v>0.198426573426573</v>
@@ -3605,10 +3662,10 @@
         <v>77</v>
       </c>
       <c r="I57" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J57" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58">
@@ -3616,13 +3673,13 @@
         <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C58" t="n">
         <v>0.527131782945736</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="E58" t="n">
         <v>0.298530954879328</v>
@@ -3637,10 +3694,10 @@
         <v>77</v>
       </c>
       <c r="I58" t="s">
-        <v>51</v>
+        <v>167</v>
       </c>
       <c r="J58" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59">
@@ -3669,10 +3726,10 @@
         <v>77</v>
       </c>
       <c r="I59" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J59" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60">
@@ -3692,7 +3749,7 @@
         <v>0.687174139728884</v>
       </c>
       <c r="F60" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G60" t="n">
         <v>0.203840806395551</v>
@@ -3701,10 +3758,10 @@
         <v>77</v>
       </c>
       <c r="I60" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J60" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61">
@@ -3715,7 +3772,7 @@
         <v>62</v>
       </c>
       <c r="C61" t="n">
-        <v>0.537414965986394</v>
+        <v>0.537414965986395</v>
       </c>
       <c r="D61" t="s">
         <v>63</v>
@@ -3730,13 +3787,13 @@
         <v>0.284896323258762</v>
       </c>
       <c r="H61" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I61" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J61" t="s">
-        <v>64</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62">
@@ -3756,7 +3813,7 @@
         <v>0.679487179487179</v>
       </c>
       <c r="F62" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G62" t="n">
         <v>0.198426573426573</v>
@@ -3765,10 +3822,10 @@
         <v>77</v>
       </c>
       <c r="I62" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J62" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63">
@@ -3797,10 +3854,10 @@
         <v>77</v>
       </c>
       <c r="I63" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J63" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64">
@@ -3808,19 +3865,19 @@
         <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="C64" t="n">
         <v>0.503703703703704</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="E64" t="n">
         <v>0.737373737373737</v>
       </c>
       <c r="F64" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="G64" t="n">
         <v>0.233670033670034</v>
@@ -3829,10 +3886,10 @@
         <v>77</v>
       </c>
       <c r="I64" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J64" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65">
@@ -3852,19 +3909,19 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G65" t="n">
         <v>0.471544715447154</v>
       </c>
       <c r="H65" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I65" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J65" t="s">
-        <v>59</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66">
@@ -3872,31 +3929,31 @@
         <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="C66" t="n">
         <v>0.377777777777778</v>
       </c>
       <c r="D66" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="E66" t="n">
         <v>0.640247859519005</v>
       </c>
       <c r="F66" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G66" t="n">
         <v>0.262470081741228</v>
       </c>
       <c r="H66" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I66" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="J66" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -3915,19 +3972,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="C1" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="D1" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="E1" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -3938,16 +3995,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="C2" t="n">
         <v>0.510666666666667</v>
       </c>
       <c r="D2" t="n">
-        <v>0.505733944954132</v>
+        <v>0.505733944954128</v>
       </c>
       <c r="E2" t="n">
-        <v>0.004932721712535</v>
+        <v>0.00493272171253822</v>
       </c>
       <c r="F2" t="s">
         <v>55</v>
@@ -3958,16 +4015,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="C3" t="n">
         <v>0.489333333333333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.494266055045875</v>
+        <v>0.494266055045872</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00493272171254155</v>
+        <v>0.00493272171253822</v>
       </c>
       <c r="F3" t="s">
         <v>55</v>
@@ -3978,16 +4035,16 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C4" t="n">
         <v>0.0766666666666667</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0791284403669724</v>
+        <v>0.0791284403669725</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00246177370030573</v>
+        <v>0.00246177370030581</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
@@ -3998,7 +4055,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="C5" t="n">
         <v>0.155333333333333</v>
@@ -4007,7 +4064,7 @@
         <v>0.10894495412844</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0463883792048932</v>
+        <v>0.0463883792048929</v>
       </c>
       <c r="F5" t="s">
         <v>55</v>
@@ -4018,16 +4075,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
         <v>0.193333333333333</v>
       </c>
       <c r="D6" t="n">
-        <v>0.134174311926605</v>
+        <v>0.134174311926606</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0591590214067282</v>
+        <v>0.0591590214067278</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -4038,7 +4095,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C7" t="n">
         <v>0.181666666666667</v>
@@ -4047,7 +4104,7 @@
         <v>0.123853211009174</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0578134556574927</v>
+        <v>0.0578134556574924</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -4058,16 +4115,16 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="C8" t="n">
         <v>0.146666666666667</v>
       </c>
       <c r="D8" t="n">
-        <v>0.122706422018348</v>
+        <v>0.122706422018349</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0239602446483184</v>
+        <v>0.023960244648318</v>
       </c>
       <c r="F8" t="s">
         <v>55</v>
@@ -4078,16 +4135,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="C9" t="n">
         <v>0.246666666666667</v>
       </c>
       <c r="D9" t="n">
-        <v>0.423165137614681</v>
+        <v>0.423165137614679</v>
       </c>
       <c r="E9" t="n">
-        <v>0.176498470948014</v>
+        <v>0.176498470948012</v>
       </c>
       <c r="F9" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Add TPS Info to TPS function
</commit_message>
<xml_diff>
--- a/CD-valid/Outcomes/Pretest/Czechia/Czechia.xlsx
+++ b/CD-valid/Outcomes/Pretest/Czechia/Czechia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="265">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -229,6 +229,12 @@
     <t xml:space="preserve">TPS_Source</t>
   </si>
   <si>
+    <t xml:space="preserve">TPS_Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS_Question</t>
+  </si>
+  <si>
     <t xml:space="preserve">Difference</t>
   </si>
   <si>
@@ -244,7 +250,13 @@
     <t xml:space="preserve">Czechia</t>
   </si>
   <si>
-    <t xml:space="preserve">Eurobarometer</t>
+    <t xml:space="preserve">Special Eurobarometer 489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q6_3. Please tell me whether the following points need to be improved in (OUR COUNTRY)?  (3) Judges are independent and are not under the influence of politicians or economic interests</t>
   </si>
   <si>
     <t xml:space="preserve">yellow</t>
@@ -262,6 +274,9 @@
     <t xml:space="preserve">SPE_489_qa6_5</t>
   </si>
   <si>
+    <t xml:space="preserve">Q6_5. Please tell me whether the following points need to be improved in (OUR COUNTRY)?  (5) Public authorities and politicians respect and apply court rulings</t>
+  </si>
+  <si>
     <t xml:space="preserve">red</t>
   </si>
   <si>
@@ -271,6 +286,15 @@
     <t xml:space="preserve">SPE_534_QA15_7</t>
   </si>
   <si>
+    <t xml:space="preserve">Special Eurobarometer SP534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA15.7. Please tell whether you agree or disagree with each of the following? :-(NATIONALITY) Government efforts to combat corruption are effective</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.03: Independent Oversight</t>
   </si>
   <si>
@@ -280,18 +304,48 @@
     <t xml:space="preserve">SPE_534_QA15_13</t>
   </si>
   <si>
+    <t xml:space="preserve">QA15.13. Please tell whether you agree or disagree with each of the following? :-In (OUR COUNTRY) measures against corruption are applied impartially and without ulterior motives</t>
+  </si>
+  <si>
     <t xml:space="preserve">green</t>
   </si>
   <si>
+    <t xml:space="preserve">Special Eurobarometer 507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QB1.4 In the context of elections in Europe, how concerned or not are you about the possibility of each of the following events?:-People being pressured into voting a particular way (M)</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.04: Elections are free, fair, and secure</t>
   </si>
   <si>
+    <t xml:space="preserve">Special Eurobarometer EB043EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA11.1. How satisfied or not are you with the following aspects of democracy in the European Union? :-Free and fair elections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q8_1. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (1) Media and journalists can criticise the government or major economic interests without risk of intimidation</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.05: Non-governmental checks</t>
   </si>
   <si>
+    <t xml:space="preserve">Q8_3. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (3) Civil society organisations and activists can operate freely and criticise the government or major economic interests without adverse consequences</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freedom in the World</t>
   </si>
   <si>
+    <t xml:space="preserve">Do the people have the right to organize in different political parties or other competitive political groupings of their choice, and is the system free of undue obstacles to the rise and fall of these competing parties or groupings?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are individuals free to express their personal views on political or other sensitive topics without fear of surveillance or retribution?</t>
+  </si>
+  <si>
     <t xml:space="preserve">PAB_emergpower</t>
   </si>
   <si>
@@ -301,6 +355,9 @@
     <t xml:space="preserve">Varieties of Democracy</t>
   </si>
   <si>
+    <t xml:space="preserve">Do members of the executive (the head of state, the head of government, and cabinet ministers) respect the constitution?</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.06: Respect for the legitimacy of the constitutional order, the law making process, and political opponents (absence of authoritarianism)</t>
   </si>
   <si>
@@ -310,6 +367,9 @@
     <t xml:space="preserve">VDM_v2juhccomp</t>
   </si>
   <si>
+    <t xml:space="preserve">How often would you say the government complies with important decisions of the high court with which it disagrees?</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.07: Respect for judicial independence (absence of authoritarianism)</t>
   </si>
   <si>
@@ -319,6 +379,9 @@
     <t xml:space="preserve">SPE_507_qb1_2</t>
   </si>
   <si>
+    <t xml:space="preserve">QB1.2 In the context of elections in Europe, how concerned or not are you about the possibility of each of the following events?:-The final result of an election being manipulated</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.09: Respect for the electoral process (absence of authoritarianism)</t>
   </si>
   <si>
@@ -328,6 +391,9 @@
     <t xml:space="preserve">VDM_v2csreprss</t>
   </si>
   <si>
+    <t xml:space="preserve">Does the government attempt to repress civil society organizations (CSOs)?</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1: Respect for civil liberties (absence of authoritarianism)</t>
   </si>
   <si>
@@ -337,12 +403,18 @@
     <t xml:space="preserve">SPE_507_qb5_2</t>
   </si>
   <si>
+    <t xml:space="preserve">QB5.2 To your knowledge, have you ever been exposed to or personally witnessed any of the following online?:-Disinformation</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL_corruption_imp</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_489_qa4_5</t>
   </si>
   <si>
+    <t xml:space="preserve">Q4_5. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (5) Corruption involving public officials and politicians is properly investigated and those responsible are brought to justice</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.11: Government officials who abuse their power are sanctioned for misconduct (accountability and sanctions for misconduct)</t>
   </si>
   <si>
@@ -352,7 +424,10 @@
     <t xml:space="preserve">GCB_Q20_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Global Corruption Barometer</t>
+    <t xml:space="preserve">Global Corruption Barometer EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q20_2. How often do you think the following situations happen in (COUNTRY)? Please tell me if you think they happen never, rarely, occasionally, often, or very often. Appropriate actions being taken against officials who engage in corruption</t>
   </si>
   <si>
     <t xml:space="preserve">1.12: Government officials who commit crimes are prosecuted and punished (accountability and sanctions for misconduct)</t>
@@ -364,6 +439,9 @@
     <t xml:space="preserve">SPE_534_QA15_4</t>
   </si>
   <si>
+    <t xml:space="preserve">QA15.4. Please tell whether you agree or disagree with each of the following? :-You are personally affected by corruption in your daily life</t>
+  </si>
+  <si>
     <t xml:space="preserve">2: Absence of Corruption</t>
   </si>
   <si>
@@ -376,12 +454,24 @@
     <t xml:space="preserve">SPE_534_QA6</t>
   </si>
   <si>
+    <t xml:space="preserve">QA6. In the past three years, would you say that the level of corruption in (OUR COUNTRY) has…?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA1. Have you been to a public healthcare practitioner such as a GP (general practitioner) or a public healthcare institution such as a public hospital in the past 12 months?/QA2. Apart from official fees did you have to give an extra payment or a valuable gift to a nurse or a doctor, or make a donation to the hospital?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q9_3. Now thinking about the same services mentioned before, how often, if ever, did you have to pay a bribe, give a gift, or do a favour in order to get the assistance or services you needed from a government office issuing official documents, such as a birth certificate, driver's licence, passport or voter's card, or a permit?</t>
+  </si>
+  <si>
     <t xml:space="preserve">ROL_abusepower_imp</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_489_qa4_4</t>
   </si>
   <si>
+    <t xml:space="preserve">Q4_4. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (4) Public officials and politicians do not use their positions to obtain benefits for themselves or their family members but take decisions in the public interest</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.4: Absence of nepotism, favoritism, and patronage</t>
   </si>
   <si>
@@ -391,12 +481,18 @@
     <t xml:space="preserve">SPE_534_QA15_11</t>
   </si>
   <si>
+    <t xml:space="preserve">QA15.11. Please tell whether you agree or disagree with each of the following? :-In (OUR COUNTRY) the only way to succeed in business is to have political connections</t>
+  </si>
+  <si>
     <t xml:space="preserve">IRE_campaign</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_534_QA15_10</t>
   </si>
   <si>
+    <t xml:space="preserve">QA15.10. Please tell whether you agree or disagree with each of the following? :-There is sufficient transparency and supervision of the financing of political parties in (OUR COUNTRY)</t>
+  </si>
+  <si>
     <t xml:space="preserve">3: Open Government</t>
   </si>
   <si>
@@ -412,24 +508,36 @@
     <t xml:space="preserve">Fundamental Rights Survey</t>
   </si>
   <si>
+    <t xml:space="preserve">Views on authorities providing information for people in a simple way</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPR_rights</t>
   </si>
   <si>
     <t xml:space="preserve">FRS_Views on authorities providing information about people's rights and entitlements</t>
   </si>
   <si>
+    <t xml:space="preserve">Views on authorities providing information about people's rights and entitlements</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPR_easy2find</t>
   </si>
   <si>
     <t xml:space="preserve">FRS_Views on authorities making information easy to find online</t>
   </si>
   <si>
+    <t xml:space="preserve">Views on authorities making information easy to find online</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPR_easy2find_online</t>
   </si>
   <si>
     <t xml:space="preserve">FRS_Views on authorities making information easy to find without using the internet</t>
   </si>
   <si>
+    <t xml:space="preserve">Views on authorities making information easy to find without using the internet</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.2: Civic participation is effectively guaranteed</t>
   </si>
   <si>
@@ -439,7 +547,13 @@
     <t xml:space="preserve">ESS_pbldmna</t>
   </si>
   <si>
-    <t xml:space="preserve">European Social Survey</t>
+    <t xml:space="preserve">The European Social Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B19-22 And still thinking about different ways of trying to improve things in [country] or help prevent things from going wrong, during the last 12 months, have you done any of the following? Have you... ...taken part in a public demonstration?</t>
   </si>
   <si>
     <t xml:space="preserve">CPA_cso</t>
@@ -448,12 +562,24 @@
     <t xml:space="preserve">ESS_volunfp</t>
   </si>
   <si>
+    <t xml:space="preserve">B19-22 And still thinking about different ways of trying to improve things in [country] or help prevent things from going wrong, during the last 12 months, have you done any of the following? Have you... ...volunteered for a not-for-profit or charitable organisation?</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRT_parliament</t>
   </si>
   <si>
     <t xml:space="preserve">ESS_trstprl</t>
   </si>
   <si>
+    <t xml:space="preserve">B6-12a Using this card, please tell me on a score of 0-10 how much you personally trust each of the institutions I read out. 0 means you do not trust an institution at all, and 10 means you have complete trust. Firstly... ...[country]'s parliament?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6-12a Using this card, please tell me on a score of 0-10 how much you personally trust each of the institutions I read out. 0 means you do not trust an institution at all, and 10 means you have complete trust. Firstly... ...the police?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6-12a Using this card, please tell me on a score of 0-10 how much you personally trust each of the institutions I read out. 0 means you do not trust an institution at all, and 10 means you have complete trust. Firstly... ...political parties?</t>
+  </si>
+  <si>
     <t xml:space="preserve">4: Fundamental Rights</t>
   </si>
   <si>
@@ -466,6 +592,9 @@
     <t xml:space="preserve">SPE_489_qa2_1</t>
   </si>
   <si>
+    <t xml:space="preserve">Q2_1. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (1) The same laws and rules apply equally to every person, including all public authorities, irrespective of their personal circumstances, social status, wealth, political connections, or origin.</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.3: Equality</t>
   </si>
   <si>
@@ -475,12 +604,21 @@
     <t xml:space="preserve">EWC_osh_risk</t>
   </si>
   <si>
+    <t xml:space="preserve">European Working Conditions Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you think your health or safety is at risk because of your work?</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.4: Solidarity</t>
   </si>
   <si>
     <t xml:space="preserve">EWC_work_life_balance</t>
   </si>
   <si>
+    <t xml:space="preserve">In general, how do your working hours fit in with your family or social commitments outside work?</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.5: Citizens' Rights</t>
   </si>
   <si>
@@ -490,6 +628,9 @@
     <t xml:space="preserve">ESS_cttresac</t>
   </si>
   <si>
+    <t xml:space="preserve">D18-21 Still using this card, please tell me to what extent you think each of the following statements applies in [country]. The courts in [country] treat everyone the same.</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.6: Justice</t>
   </si>
   <si>
@@ -499,6 +640,12 @@
     <t xml:space="preserve">SPE_489_qa5_1</t>
   </si>
   <si>
+    <t xml:space="preserve">Q5_1. How important for you personally are the following points? (1) If your rights are not respected, you can have them upheld by an independent court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does due process prevail in civil and criminal matters?</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEC_orgcrime</t>
   </si>
   <si>
@@ -508,6 +655,9 @@
     <t xml:space="preserve">Organized Crime Index</t>
   </si>
   <si>
+    <t xml:space="preserve">Criminality average score</t>
+  </si>
+  <si>
     <t xml:space="preserve">5: Order and Security</t>
   </si>
   <si>
@@ -529,18 +679,27 @@
     <t xml:space="preserve">VDM_v2clacjstm</t>
   </si>
   <si>
+    <t xml:space="preserve">Do men enjoy secure and effective access to justice?</t>
+  </si>
+  <si>
     <t xml:space="preserve">7.2: People can access quality legal assistance and representation</t>
   </si>
   <si>
     <t xml:space="preserve">VDM_v2clacjstw</t>
   </si>
   <si>
+    <t xml:space="preserve">Do women enjoy equal, secure, and effective access to justice?</t>
+  </si>
+  <si>
     <t xml:space="preserve">JSE_affordcosts</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_489_qa5_2</t>
   </si>
   <si>
+    <t xml:space="preserve">Q5_2. How important for you personally are the following points? (2) Court proceedings are not excessively long or costly</t>
+  </si>
+  <si>
     <t xml:space="preserve">7.3: Civil justice is people-centered, accessible, efficient, and outcome-oriented</t>
   </si>
   <si>
@@ -550,21 +709,36 @@
     <t xml:space="preserve">7.4: Civil justice is impartial and free from corruption and undue influence</t>
   </si>
   <si>
+    <t xml:space="preserve">Q5_7. How many of the following people in (COUNTRY) do you think are involved in corruption? Please tell me if you think it is none of them, some of them, most of them, or all of them. Judges and magistrates</t>
+  </si>
+  <si>
     <t xml:space="preserve">JSE_enforce</t>
   </si>
   <si>
     <t xml:space="preserve">SPE_489_qa6_1</t>
   </si>
   <si>
+    <t xml:space="preserve">Q6_1. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (1) If your rights are not respected, you can have them upheld by an independent court</t>
+  </si>
+  <si>
     <t xml:space="preserve">7.5: Civil justice is effectively enforced</t>
   </si>
   <si>
+    <t xml:space="preserve">Q6_4. Please tell me whether the following points need to be improved in (OUR COUNTRY)? (4) The police and prosecution service investigate crimes properly including those committed by politicians or influential persons and they are not under the influence of politicians or economic interests</t>
+  </si>
+  <si>
     <t xml:space="preserve">8: Criminal Justice</t>
   </si>
   <si>
     <t xml:space="preserve">8.1: Criminal Investigation</t>
   </si>
   <si>
+    <t xml:space="preserve">Q5_6. How many of the following people in (COUNTRY) do you think are involved in corruption? Please tell me if you think it is none of them, some of them, most of them, or all of them. Police</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5_4. How important for you personally are the following points? (4) The police and prosecution service investigate crimes properly including those committed by politicians or influential persons and they are not under the influence of politicians or economic interests</t>
+  </si>
+  <si>
     <t xml:space="preserve">8.2: Prosecution and pre-trial process</t>
   </si>
   <si>
@@ -577,6 +751,9 @@
     <t xml:space="preserve">FRS_Perception of the way the police generally treats people</t>
   </si>
   <si>
+    <t xml:space="preserve">Perception of the way the police generally treats people</t>
+  </si>
+  <si>
     <t xml:space="preserve">8.5: Victim's Rights</t>
   </si>
   <si>
@@ -587,6 +764,9 @@
   </si>
   <si>
     <t xml:space="preserve">VDM_v2cltort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there freedom from torture?</t>
   </si>
   <si>
     <t xml:space="preserve">8.7: Prisons</t>
@@ -1875,10 +2055,16 @@
       <c r="J1" t="s">
         <v>74</v>
       </c>
+      <c r="K1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1893,120 +2079,144 @@
         <v>0.247946611909651</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" t="n">
+        <v>78</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="n">
         <v>0.218720054757016</v>
       </c>
-      <c r="H2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" t="s">
-        <v>78</v>
-      </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C3" t="n">
         <v>0.569444444444444</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E3" t="n">
         <v>0.260980592441267</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="n">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="n">
         <v>0.308463852003178</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" t="s">
         <v>82</v>
       </c>
-      <c r="I3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" t="s">
-        <v>79</v>
+      <c r="L3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C4" t="n">
         <v>0.479674796747967</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E4" t="n">
         <v>0.679902473005921</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" t="n">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.200227676257954</v>
       </c>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" t="s">
-        <v>78</v>
-      </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="K4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C5" t="n">
         <v>0.527131782945736</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E5" t="n">
         <v>0.608050019538882</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" t="n">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" t="n">
         <v>0.080918236593146</v>
       </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2021,24 +2231,30 @@
         <v>0.279047619047619</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" t="n">
+        <v>98</v>
+      </c>
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" t="n">
         <v>0.235445134575569</v>
       </c>
-      <c r="H6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I6" t="s">
-        <v>78</v>
-      </c>
       <c r="J6" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -2053,24 +2269,30 @@
         <v>0.598632478632479</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" t="n">
+        <v>102</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.0884283969998255</v>
       </c>
-      <c r="H7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" t="s">
-        <v>78</v>
-      </c>
       <c r="J7" t="s">
-        <v>89</v>
+        <v>97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -2085,24 +2307,30 @@
         <v>0.389296956977964</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" t="n">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" t="n">
         <v>0.177369709688702</v>
       </c>
-      <c r="H8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I8" t="s">
-        <v>78</v>
-      </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="K8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -2117,24 +2345,30 @@
         <v>0.413774973711882</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" t="n">
+        <v>78</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" t="n">
         <v>0.0252494165320202</v>
       </c>
-      <c r="H9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" t="s">
-        <v>78</v>
-      </c>
       <c r="J9" t="s">
-        <v>90</v>
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
@@ -2149,24 +2383,30 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s">
         <v>91</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" t="n">
         <v>0.425</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" t="s">
         <v>82</v>
       </c>
-      <c r="I10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" t="s">
-        <v>90</v>
+      <c r="L10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -2181,312 +2421,372 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
         <v>91</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.495495495495496</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" t="s">
         <v>82</v>
       </c>
-      <c r="I11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" t="s">
-        <v>90</v>
+      <c r="L11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C12" t="n">
         <v>0.577777777777778</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="E12" t="n">
         <v>0.483167782183002</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" t="n">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" t="n">
         <v>0.0946099955947761</v>
       </c>
-      <c r="H12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" t="s">
-        <v>78</v>
-      </c>
       <c r="J12" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+      <c r="K12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C13" t="n">
         <v>0.5</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="E13" t="n">
         <v>0.509136975455265</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" t="n">
+        <v>112</v>
+      </c>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" t="n">
         <v>0.00913697545526526</v>
       </c>
-      <c r="H13" t="s">
-        <v>88</v>
-      </c>
-      <c r="I13" t="s">
-        <v>78</v>
-      </c>
       <c r="J13" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="K13" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C14" t="n">
         <v>0.558823529411765</v>
       </c>
       <c r="D14" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E14" t="n">
         <v>0.28757546870035</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" t="n">
+        <v>98</v>
+      </c>
+      <c r="G14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" t="n">
         <v>0.271248060711415</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K14" t="s">
         <v>82</v>
       </c>
-      <c r="I14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" t="s">
-        <v>101</v>
+      <c r="L14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="C15" t="n">
         <v>0.530612244897959</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="E15" t="n">
         <v>0.611451306841004</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
-      </c>
-      <c r="G15" t="n">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.0808390619430452</v>
       </c>
-      <c r="H15" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" t="s">
-        <v>78</v>
-      </c>
       <c r="J15" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="K15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="C16" t="n">
         <v>0.412698412698413</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E16" t="n">
         <v>0.22952380952381</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" t="n">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.183174603174603</v>
       </c>
-      <c r="H16" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" t="s">
-        <v>78</v>
-      </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>81</v>
+      </c>
+      <c r="K16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="C17" t="n">
         <v>0.487341772151899</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="E17" t="n">
         <v>0.131155778894472</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" t="n">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" t="n">
         <v>0.356185993257426</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" t="s">
         <v>82</v>
       </c>
-      <c r="I17" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" t="s">
-        <v>109</v>
+      <c r="L17" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C18" t="n">
         <v>0.517543859649123</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="E18" t="n">
         <v>0.422395273899033</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" t="n">
+        <v>136</v>
+      </c>
+      <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.0951485857500894</v>
       </c>
-      <c r="H18" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" t="s">
-        <v>78</v>
-      </c>
       <c r="J18" t="s">
-        <v>113</v>
+        <v>97</v>
+      </c>
+      <c r="K18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L18" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="C19" t="n">
         <v>0.514767932489451</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="E19" t="n">
         <v>0.755873340143003</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" t="n">
+        <v>90</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" t="n">
         <v>0.241105407653552</v>
       </c>
-      <c r="H19" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" t="s">
-        <v>116</v>
-      </c>
       <c r="J19" t="s">
-        <v>117</v>
+        <v>81</v>
+      </c>
+      <c r="K19" t="s">
+        <v>142</v>
+      </c>
+      <c r="L19" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="C20" t="n">
         <v>0.478658536585366</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="E20" t="n">
         <v>0.391025641025641</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" t="n">
+        <v>90</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" t="s">
+        <v>146</v>
+      </c>
+      <c r="I20" t="n">
         <v>0.0876328955597248</v>
       </c>
-      <c r="H20" t="s">
-        <v>88</v>
-      </c>
-      <c r="I20" t="s">
-        <v>116</v>
-      </c>
       <c r="J20" t="s">
-        <v>117</v>
+        <v>97</v>
+      </c>
+      <c r="K20" t="s">
+        <v>142</v>
+      </c>
+      <c r="L20" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -2501,24 +2801,30 @@
         <v>0.949004975124378</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" t="n">
+        <v>90</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" t="n">
         <v>0.699004975124378</v>
       </c>
-      <c r="H21" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" t="s">
-        <v>116</v>
-      </c>
       <c r="J21" t="s">
-        <v>117</v>
+        <v>87</v>
+      </c>
+      <c r="K21" t="s">
+        <v>142</v>
+      </c>
+      <c r="L21" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
@@ -2533,248 +2839,296 @@
         <v>0.0218446601941748</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" t="n">
+        <v>136</v>
+      </c>
+      <c r="G22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" t="n">
         <v>0.603155339805825</v>
       </c>
-      <c r="H22" t="s">
-        <v>82</v>
-      </c>
-      <c r="I22" t="s">
-        <v>116</v>
-      </c>
       <c r="J22" t="s">
-        <v>117</v>
+        <v>87</v>
+      </c>
+      <c r="K22" t="s">
+        <v>142</v>
+      </c>
+      <c r="L22" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="C23" t="n">
         <v>0.449367088607595</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
       <c r="E23" t="n">
         <v>0.175200803212851</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" t="n">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
+        <v>79</v>
+      </c>
+      <c r="H23" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.274166285394744</v>
       </c>
-      <c r="H23" t="s">
-        <v>82</v>
-      </c>
-      <c r="I23" t="s">
-        <v>116</v>
-      </c>
       <c r="J23" t="s">
-        <v>122</v>
+        <v>87</v>
+      </c>
+      <c r="K23" t="s">
+        <v>142</v>
+      </c>
+      <c r="L23" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="C24" t="n">
         <v>0.57088122605364</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E24" t="n">
         <v>0.52060737527115</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" t="n">
+        <v>90</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" t="n">
         <v>0.0502738507824901</v>
       </c>
-      <c r="H24" t="s">
-        <v>88</v>
-      </c>
-      <c r="I24" t="s">
-        <v>116</v>
-      </c>
       <c r="J24" t="s">
-        <v>122</v>
+        <v>97</v>
+      </c>
+      <c r="K24" t="s">
+        <v>142</v>
+      </c>
+      <c r="L24" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="C25" t="n">
         <v>0.488636363636364</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="E25" t="n">
         <v>0.643249176728869</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" t="n">
+        <v>90</v>
+      </c>
+      <c r="G25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" t="n">
         <v>0.154612813092506</v>
       </c>
-      <c r="H25" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" t="s">
-        <v>127</v>
-      </c>
       <c r="J25" t="s">
-        <v>128</v>
+        <v>81</v>
+      </c>
+      <c r="K25" t="s">
+        <v>159</v>
+      </c>
+      <c r="L25" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="C26" t="n">
         <v>0.542635658914729</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="E26" t="n">
         <v>0.752525252525253</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" t="n">
+        <v>163</v>
+      </c>
+      <c r="G26" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" t="s">
+        <v>164</v>
+      </c>
+      <c r="I26" t="n">
         <v>0.209889593610524</v>
       </c>
-      <c r="H26" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" t="s">
-        <v>127</v>
-      </c>
       <c r="J26" t="s">
-        <v>128</v>
+        <v>81</v>
+      </c>
+      <c r="K26" t="s">
+        <v>159</v>
+      </c>
+      <c r="L26" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="C27" t="n">
         <v>0.546511627906977</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="E27" t="n">
         <v>0.686868686868687</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
-      </c>
-      <c r="G27" t="n">
+        <v>163</v>
+      </c>
+      <c r="G27" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I27" t="n">
         <v>0.14035705896171</v>
       </c>
-      <c r="H27" t="s">
-        <v>77</v>
-      </c>
-      <c r="I27" t="s">
-        <v>127</v>
-      </c>
       <c r="J27" t="s">
-        <v>128</v>
+        <v>81</v>
+      </c>
+      <c r="K27" t="s">
+        <v>159</v>
+      </c>
+      <c r="L27" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C28" t="n">
         <v>0.491452991452991</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="E28" t="n">
         <v>0.752577319587629</v>
       </c>
       <c r="F28" t="s">
-        <v>131</v>
-      </c>
-      <c r="G28" t="n">
+        <v>163</v>
+      </c>
+      <c r="G28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" t="s">
+        <v>170</v>
+      </c>
+      <c r="I28" t="n">
         <v>0.261124328134637</v>
       </c>
-      <c r="H28" t="s">
-        <v>82</v>
-      </c>
-      <c r="I28" t="s">
-        <v>127</v>
-      </c>
       <c r="J28" t="s">
-        <v>128</v>
+        <v>87</v>
+      </c>
+      <c r="K28" t="s">
+        <v>159</v>
+      </c>
+      <c r="L28" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="C29" t="n">
         <v>0.524390243902439</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="E29" t="n">
         <v>0.622448979591837</v>
       </c>
       <c r="F29" t="s">
-        <v>131</v>
-      </c>
-      <c r="G29" t="n">
+        <v>163</v>
+      </c>
+      <c r="G29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" t="s">
+        <v>173</v>
+      </c>
+      <c r="I29" t="n">
         <v>0.0980587356893977</v>
       </c>
-      <c r="H29" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" t="s">
-        <v>127</v>
-      </c>
       <c r="J29" t="s">
-        <v>128</v>
+        <v>97</v>
+      </c>
+      <c r="K29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L29" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -2789,24 +3143,30 @@
         <v>0.389296956977964</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
-      </c>
-      <c r="G30" t="n">
+        <v>78</v>
+      </c>
+      <c r="G30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" t="s">
+        <v>104</v>
+      </c>
+      <c r="I30" t="n">
         <v>0.177369709688702</v>
       </c>
-      <c r="H30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I30" t="s">
-        <v>127</v>
-      </c>
       <c r="J30" t="s">
-        <v>138</v>
+        <v>81</v>
+      </c>
+      <c r="K30" t="s">
+        <v>159</v>
+      </c>
+      <c r="L30" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
         <v>25</v>
@@ -2821,24 +3181,30 @@
         <v>0.413774973711882</v>
       </c>
       <c r="F31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" t="n">
+        <v>78</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" t="n">
         <v>0.0252494165320202</v>
       </c>
-      <c r="H31" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" t="s">
-        <v>127</v>
-      </c>
       <c r="J31" t="s">
-        <v>138</v>
+        <v>97</v>
+      </c>
+      <c r="K31" t="s">
+        <v>159</v>
+      </c>
+      <c r="L31" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
         <v>21</v>
@@ -2853,24 +3219,30 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" t="s">
         <v>91</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="s">
+        <v>108</v>
+      </c>
+      <c r="I32" t="n">
         <v>0.425</v>
       </c>
-      <c r="H32" t="s">
-        <v>82</v>
-      </c>
-      <c r="I32" t="s">
-        <v>127</v>
-      </c>
       <c r="J32" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="K32" t="s">
+        <v>159</v>
+      </c>
+      <c r="L32" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -2885,120 +3257,144 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" t="s">
         <v>91</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" t="n">
         <v>0.495495495495496</v>
       </c>
-      <c r="H33" t="s">
-        <v>82</v>
-      </c>
-      <c r="I33" t="s">
-        <v>127</v>
-      </c>
       <c r="J33" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="K33" t="s">
+        <v>159</v>
+      </c>
+      <c r="L33" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="C34" t="n">
         <v>0.5</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="E34" t="n">
         <v>0.0628803245436105</v>
       </c>
       <c r="F34" t="s">
-        <v>141</v>
-      </c>
-      <c r="G34" t="n">
+        <v>177</v>
+      </c>
+      <c r="G34" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" t="s">
+        <v>179</v>
+      </c>
+      <c r="I34" t="n">
         <v>0.437119675456389</v>
       </c>
-      <c r="H34" t="s">
-        <v>82</v>
-      </c>
-      <c r="I34" t="s">
-        <v>127</v>
-      </c>
       <c r="J34" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="K34" t="s">
+        <v>159</v>
+      </c>
+      <c r="L34" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="C35" t="n">
         <v>0.419354838709677</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="E35" t="n">
         <v>0.0568412505075112</v>
       </c>
       <c r="F35" t="s">
-        <v>141</v>
-      </c>
-      <c r="G35" t="n">
+        <v>177</v>
+      </c>
+      <c r="G35" t="s">
+        <v>178</v>
+      </c>
+      <c r="H35" t="s">
+        <v>182</v>
+      </c>
+      <c r="I35" t="n">
         <v>0.362513588202166</v>
       </c>
-      <c r="H35" t="s">
-        <v>82</v>
-      </c>
-      <c r="I35" t="s">
-        <v>127</v>
-      </c>
       <c r="J35" t="s">
-        <v>138</v>
+        <v>87</v>
+      </c>
+      <c r="K35" t="s">
+        <v>159</v>
+      </c>
+      <c r="L35" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="C36" t="n">
         <v>0.478927203065134</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="E36" t="n">
         <v>0.468680182043856</v>
       </c>
       <c r="F36" t="s">
-        <v>141</v>
-      </c>
-      <c r="G36" t="n">
+        <v>177</v>
+      </c>
+      <c r="G36" t="s">
+        <v>178</v>
+      </c>
+      <c r="H36" t="s">
+        <v>185</v>
+      </c>
+      <c r="I36" t="n">
         <v>0.0102470210212781</v>
       </c>
-      <c r="H36" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" t="s">
-        <v>127</v>
-      </c>
       <c r="J36" t="s">
-        <v>138</v>
+        <v>97</v>
+      </c>
+      <c r="K36" t="s">
+        <v>159</v>
+      </c>
+      <c r="L36" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
@@ -3013,24 +3409,30 @@
         <v>0.644869706840391</v>
       </c>
       <c r="F37" t="s">
-        <v>141</v>
-      </c>
-      <c r="G37" t="n">
+        <v>177</v>
+      </c>
+      <c r="G37" t="s">
+        <v>178</v>
+      </c>
+      <c r="H37" t="s">
+        <v>186</v>
+      </c>
+      <c r="I37" t="n">
         <v>0.126351188321872</v>
       </c>
-      <c r="H37" t="s">
-        <v>77</v>
-      </c>
-      <c r="I37" t="s">
-        <v>127</v>
-      </c>
       <c r="J37" t="s">
-        <v>138</v>
+        <v>81</v>
+      </c>
+      <c r="K37" t="s">
+        <v>159</v>
+      </c>
+      <c r="L37" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
@@ -3045,24 +3447,30 @@
         <v>0.383012689316414</v>
       </c>
       <c r="F38" t="s">
-        <v>141</v>
-      </c>
-      <c r="G38" t="n">
+        <v>177</v>
+      </c>
+      <c r="G38" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" t="s">
+        <v>187</v>
+      </c>
+      <c r="I38" t="n">
         <v>0.0128206440169191</v>
       </c>
-      <c r="H38" t="s">
-        <v>88</v>
-      </c>
-      <c r="I38" t="s">
-        <v>127</v>
-      </c>
       <c r="J38" t="s">
-        <v>138</v>
+        <v>97</v>
+      </c>
+      <c r="K38" t="s">
+        <v>159</v>
+      </c>
+      <c r="L38" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
@@ -3077,24 +3485,30 @@
         <v>0.389296956977964</v>
       </c>
       <c r="F39" t="s">
-        <v>76</v>
-      </c>
-      <c r="G39" t="n">
+        <v>78</v>
+      </c>
+      <c r="G39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H39" t="s">
+        <v>104</v>
+      </c>
+      <c r="I39" t="n">
         <v>0.177369709688702</v>
       </c>
-      <c r="H39" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" t="s">
-        <v>146</v>
-      </c>
       <c r="J39" t="s">
-        <v>147</v>
+        <v>81</v>
+      </c>
+      <c r="K39" t="s">
+        <v>188</v>
+      </c>
+      <c r="L39" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
@@ -3109,24 +3523,30 @@
         <v>0.413774973711882</v>
       </c>
       <c r="F40" t="s">
-        <v>76</v>
-      </c>
-      <c r="G40" t="n">
+        <v>78</v>
+      </c>
+      <c r="G40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" t="s">
+        <v>106</v>
+      </c>
+      <c r="I40" t="n">
         <v>0.0252494165320202</v>
       </c>
-      <c r="H40" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" t="s">
-        <v>146</v>
-      </c>
       <c r="J40" t="s">
-        <v>147</v>
+        <v>97</v>
+      </c>
+      <c r="K40" t="s">
+        <v>188</v>
+      </c>
+      <c r="L40" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
         <v>21</v>
@@ -3141,24 +3561,30 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" t="s">
         <v>91</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" t="n">
         <v>0.425</v>
       </c>
-      <c r="H41" t="s">
-        <v>82</v>
-      </c>
-      <c r="I41" t="s">
-        <v>146</v>
-      </c>
       <c r="J41" t="s">
-        <v>147</v>
+        <v>87</v>
+      </c>
+      <c r="K41" t="s">
+        <v>188</v>
+      </c>
+      <c r="L41" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
@@ -3173,120 +3599,144 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" t="s">
         <v>91</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" t="n">
         <v>0.495495495495496</v>
       </c>
-      <c r="H42" t="s">
-        <v>82</v>
-      </c>
-      <c r="I42" t="s">
-        <v>146</v>
-      </c>
       <c r="J42" t="s">
-        <v>147</v>
+        <v>87</v>
+      </c>
+      <c r="K42" t="s">
+        <v>188</v>
+      </c>
+      <c r="L42" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="C43" t="n">
         <v>0.529069767441861</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="E43" t="n">
         <v>0.196446700507614</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
-      </c>
-      <c r="G43" t="n">
+        <v>78</v>
+      </c>
+      <c r="G43" t="s">
+        <v>79</v>
+      </c>
+      <c r="H43" t="s">
+        <v>192</v>
+      </c>
+      <c r="I43" t="n">
         <v>0.332623066934246</v>
       </c>
-      <c r="H43" t="s">
-        <v>82</v>
-      </c>
-      <c r="I43" t="s">
-        <v>146</v>
-      </c>
       <c r="J43" t="s">
-        <v>150</v>
+        <v>87</v>
+      </c>
+      <c r="K43" t="s">
+        <v>188</v>
+      </c>
+      <c r="L43" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="C44" t="n">
         <v>0.591666666666667</v>
       </c>
       <c r="D44" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="E44" t="n">
         <v>0.752525252525252</v>
       </c>
       <c r="F44" t="s">
-        <v>76</v>
-      </c>
-      <c r="G44" t="n">
+        <v>196</v>
+      </c>
+      <c r="G44" t="s">
+        <v>99</v>
+      </c>
+      <c r="H44" t="s">
+        <v>197</v>
+      </c>
+      <c r="I44" t="n">
         <v>0.160858585858586</v>
       </c>
-      <c r="H44" t="s">
-        <v>77</v>
-      </c>
-      <c r="I44" t="s">
-        <v>146</v>
-      </c>
       <c r="J44" t="s">
-        <v>153</v>
+        <v>81</v>
+      </c>
+      <c r="K44" t="s">
+        <v>188</v>
+      </c>
+      <c r="L44" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="C45" t="n">
         <v>0.591666666666667</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
       <c r="E45" t="n">
         <v>0.688676075268817</v>
       </c>
       <c r="F45" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" t="n">
+        <v>196</v>
+      </c>
+      <c r="G45" t="s">
+        <v>99</v>
+      </c>
+      <c r="H45" t="s">
+        <v>200</v>
+      </c>
+      <c r="I45" t="n">
         <v>0.0970094086021505</v>
       </c>
-      <c r="H45" t="s">
-        <v>88</v>
-      </c>
-      <c r="I45" t="s">
-        <v>146</v>
-      </c>
       <c r="J45" t="s">
-        <v>153</v>
+        <v>97</v>
+      </c>
+      <c r="K45" t="s">
+        <v>188</v>
+      </c>
+      <c r="L45" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
@@ -3301,88 +3751,106 @@
         <v>0.279047619047619</v>
       </c>
       <c r="F46" t="s">
-        <v>76</v>
-      </c>
-      <c r="G46" t="n">
+        <v>98</v>
+      </c>
+      <c r="G46" t="s">
+        <v>99</v>
+      </c>
+      <c r="H46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I46" t="n">
         <v>0.235445134575569</v>
       </c>
-      <c r="H46" t="s">
-        <v>77</v>
-      </c>
-      <c r="I46" t="s">
-        <v>146</v>
-      </c>
       <c r="J46" t="s">
-        <v>155</v>
+        <v>81</v>
+      </c>
+      <c r="K46" t="s">
+        <v>188</v>
+      </c>
+      <c r="L46" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>156</v>
+        <v>202</v>
       </c>
       <c r="C47" t="n">
         <v>0.418439716312057</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="E47" t="n">
         <v>0.53935860058309</v>
       </c>
       <c r="F47" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" t="n">
+        <v>177</v>
+      </c>
+      <c r="G47" t="s">
+        <v>178</v>
+      </c>
+      <c r="H47" t="s">
+        <v>204</v>
+      </c>
+      <c r="I47" t="n">
         <v>0.120918884271034</v>
       </c>
-      <c r="H47" t="s">
-        <v>77</v>
-      </c>
-      <c r="I47" t="s">
-        <v>146</v>
-      </c>
       <c r="J47" t="s">
-        <v>158</v>
+        <v>81</v>
+      </c>
+      <c r="K47" t="s">
+        <v>188</v>
+      </c>
+      <c r="L47" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C48" t="n">
         <v>0.486842105263158</v>
       </c>
       <c r="D48" t="s">
-        <v>160</v>
+        <v>207</v>
       </c>
       <c r="E48" t="n">
         <v>0.763299663299663</v>
       </c>
       <c r="F48" t="s">
-        <v>76</v>
-      </c>
-      <c r="G48" t="n">
+        <v>78</v>
+      </c>
+      <c r="G48" t="s">
+        <v>79</v>
+      </c>
+      <c r="H48" t="s">
+        <v>208</v>
+      </c>
+      <c r="I48" t="n">
         <v>0.276457558036505</v>
       </c>
-      <c r="H48" t="s">
-        <v>82</v>
-      </c>
-      <c r="I48" t="s">
-        <v>146</v>
-      </c>
       <c r="J48" t="s">
-        <v>158</v>
+        <v>87</v>
+      </c>
+      <c r="K48" t="s">
+        <v>188</v>
+      </c>
+      <c r="L48" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
         <v>45</v>
@@ -3397,216 +3865,258 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49" t="s">
         <v>91</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="s">
+        <v>209</v>
+      </c>
+      <c r="I49" t="n">
         <v>0.484848484848485</v>
       </c>
-      <c r="H49" t="s">
-        <v>82</v>
-      </c>
-      <c r="I49" t="s">
-        <v>146</v>
-      </c>
       <c r="J49" t="s">
-        <v>158</v>
+        <v>87</v>
+      </c>
+      <c r="K49" t="s">
+        <v>188</v>
+      </c>
+      <c r="L49" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
       <c r="C50" t="n">
         <v>0.431034482758621</v>
       </c>
       <c r="D50" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="E50" t="n">
         <v>0.591111111111111</v>
       </c>
       <c r="F50" t="s">
-        <v>163</v>
-      </c>
-      <c r="G50" t="n">
+        <v>212</v>
+      </c>
+      <c r="G50" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50" t="s">
+        <v>213</v>
+      </c>
+      <c r="I50" t="n">
         <v>0.16007662835249</v>
       </c>
-      <c r="H50" t="s">
-        <v>77</v>
-      </c>
-      <c r="I50" t="s">
-        <v>164</v>
-      </c>
       <c r="J50" t="s">
-        <v>165</v>
+        <v>81</v>
+      </c>
+      <c r="K50" t="s">
+        <v>214</v>
+      </c>
+      <c r="L50" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="C51" t="n">
         <v>0.446808510638298</v>
       </c>
       <c r="D51" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="E51" t="n">
         <v>0.752525252525253</v>
       </c>
       <c r="F51" t="s">
-        <v>131</v>
-      </c>
-      <c r="G51" t="n">
+        <v>163</v>
+      </c>
+      <c r="G51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H51" t="s">
+        <v>164</v>
+      </c>
+      <c r="I51" t="n">
         <v>0.305716741886955</v>
       </c>
-      <c r="H51" t="s">
-        <v>82</v>
-      </c>
-      <c r="I51" t="s">
-        <v>167</v>
-      </c>
       <c r="J51" t="s">
-        <v>168</v>
+        <v>87</v>
+      </c>
+      <c r="K51" t="s">
+        <v>217</v>
+      </c>
+      <c r="L51" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="C52" t="n">
         <v>0.503875968992248</v>
       </c>
       <c r="D52" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="E52" t="n">
         <v>0.548034598454766</v>
       </c>
       <c r="F52" t="s">
-        <v>94</v>
-      </c>
-      <c r="G52" t="n">
+        <v>112</v>
+      </c>
+      <c r="G52" t="s">
+        <v>91</v>
+      </c>
+      <c r="H52" t="s">
+        <v>221</v>
+      </c>
+      <c r="I52" t="n">
         <v>0.0441586294625184</v>
       </c>
-      <c r="H52" t="s">
-        <v>88</v>
-      </c>
-      <c r="I52" t="s">
-        <v>167</v>
-      </c>
       <c r="J52" t="s">
-        <v>171</v>
+        <v>97</v>
+      </c>
+      <c r="K52" t="s">
+        <v>217</v>
+      </c>
+      <c r="L52" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="C53" t="n">
         <v>0.503875968992248</v>
       </c>
       <c r="D53" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="E53" t="n">
         <v>0.497777444253569</v>
       </c>
       <c r="F53" t="s">
-        <v>94</v>
-      </c>
-      <c r="G53" t="n">
+        <v>112</v>
+      </c>
+      <c r="G53" t="s">
+        <v>91</v>
+      </c>
+      <c r="H53" t="s">
+        <v>224</v>
+      </c>
+      <c r="I53" t="n">
         <v>0.00609852473867861</v>
       </c>
-      <c r="H53" t="s">
-        <v>88</v>
-      </c>
-      <c r="I53" t="s">
-        <v>167</v>
-      </c>
       <c r="J53" t="s">
-        <v>171</v>
+        <v>97</v>
+      </c>
+      <c r="K53" t="s">
+        <v>217</v>
+      </c>
+      <c r="L53" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="C54" t="n">
         <v>0.486111111111111</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
       <c r="E54" t="n">
         <v>0.772018970189702</v>
       </c>
       <c r="F54" t="s">
-        <v>76</v>
-      </c>
-      <c r="G54" t="n">
+        <v>78</v>
+      </c>
+      <c r="G54" t="s">
+        <v>79</v>
+      </c>
+      <c r="H54" t="s">
+        <v>227</v>
+      </c>
+      <c r="I54" t="n">
         <v>0.285907859078591</v>
       </c>
-      <c r="H54" t="s">
-        <v>82</v>
-      </c>
-      <c r="I54" t="s">
-        <v>167</v>
-      </c>
       <c r="J54" t="s">
-        <v>175</v>
+        <v>87</v>
+      </c>
+      <c r="K54" t="s">
+        <v>217</v>
+      </c>
+      <c r="L54" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>176</v>
+        <v>229</v>
       </c>
       <c r="C55" t="n">
         <v>0.526666666666667</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>226</v>
       </c>
       <c r="E55" t="n">
         <v>0.772018970189702</v>
       </c>
       <c r="F55" t="s">
-        <v>76</v>
-      </c>
-      <c r="G55" t="n">
+        <v>78</v>
+      </c>
+      <c r="G55" t="s">
+        <v>79</v>
+      </c>
+      <c r="H55" t="s">
+        <v>227</v>
+      </c>
+      <c r="I55" t="n">
         <v>0.245352303523035</v>
       </c>
-      <c r="H55" t="s">
-        <v>77</v>
-      </c>
-      <c r="I55" t="s">
-        <v>167</v>
-      </c>
       <c r="J55" t="s">
-        <v>175</v>
+        <v>81</v>
+      </c>
+      <c r="K55" t="s">
+        <v>217</v>
+      </c>
+      <c r="L55" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
         <v>27</v>
@@ -3621,24 +4131,30 @@
         <v>0.247946611909651</v>
       </c>
       <c r="F56" t="s">
-        <v>76</v>
-      </c>
-      <c r="G56" t="n">
+        <v>78</v>
+      </c>
+      <c r="G56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I56" t="n">
         <v>0.218720054757016</v>
       </c>
-      <c r="H56" t="s">
-        <v>77</v>
-      </c>
-      <c r="I56" t="s">
-        <v>167</v>
-      </c>
       <c r="J56" t="s">
-        <v>177</v>
+        <v>81</v>
+      </c>
+      <c r="K56" t="s">
+        <v>217</v>
+      </c>
+      <c r="L56" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
         <v>48</v>
@@ -3653,56 +4169,68 @@
         <v>0.679487179487179</v>
       </c>
       <c r="F57" t="s">
-        <v>112</v>
-      </c>
-      <c r="G57" t="n">
+        <v>136</v>
+      </c>
+      <c r="G57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H57" t="s">
+        <v>231</v>
+      </c>
+      <c r="I57" t="n">
         <v>0.198426573426573</v>
       </c>
-      <c r="H57" t="s">
-        <v>77</v>
-      </c>
-      <c r="I57" t="s">
-        <v>167</v>
-      </c>
       <c r="J57" t="s">
-        <v>177</v>
+        <v>81</v>
+      </c>
+      <c r="K57" t="s">
+        <v>217</v>
+      </c>
+      <c r="L57" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>178</v>
+        <v>232</v>
       </c>
       <c r="C58" t="n">
         <v>0.527131782945736</v>
       </c>
       <c r="D58" t="s">
-        <v>179</v>
+        <v>233</v>
       </c>
       <c r="E58" t="n">
         <v>0.298530954879328</v>
       </c>
       <c r="F58" t="s">
-        <v>76</v>
-      </c>
-      <c r="G58" t="n">
+        <v>78</v>
+      </c>
+      <c r="G58" t="s">
+        <v>79</v>
+      </c>
+      <c r="H58" t="s">
+        <v>234</v>
+      </c>
+      <c r="I58" t="n">
         <v>0.228600828066408</v>
       </c>
-      <c r="H58" t="s">
-        <v>77</v>
-      </c>
-      <c r="I58" t="s">
-        <v>167</v>
-      </c>
       <c r="J58" t="s">
-        <v>180</v>
+        <v>81</v>
+      </c>
+      <c r="K58" t="s">
+        <v>217</v>
+      </c>
+      <c r="L58" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
         <v>60</v>
@@ -3717,24 +4245,30 @@
         <v>0.193711967545639</v>
       </c>
       <c r="F59" t="s">
-        <v>76</v>
-      </c>
-      <c r="G59" t="n">
+        <v>78</v>
+      </c>
+      <c r="G59" t="s">
+        <v>79</v>
+      </c>
+      <c r="H59" t="s">
+        <v>236</v>
+      </c>
+      <c r="I59" t="n">
         <v>0.229899143565472</v>
       </c>
-      <c r="H59" t="s">
-        <v>77</v>
-      </c>
-      <c r="I59" t="s">
-        <v>181</v>
-      </c>
       <c r="J59" t="s">
-        <v>182</v>
+        <v>81</v>
+      </c>
+      <c r="K59" t="s">
+        <v>237</v>
+      </c>
+      <c r="L59" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
         <v>54</v>
@@ -3749,24 +4283,30 @@
         <v>0.687174139728884</v>
       </c>
       <c r="F60" t="s">
-        <v>112</v>
-      </c>
-      <c r="G60" t="n">
+        <v>136</v>
+      </c>
+      <c r="G60" t="s">
+        <v>99</v>
+      </c>
+      <c r="H60" t="s">
+        <v>239</v>
+      </c>
+      <c r="I60" t="n">
         <v>0.203840806395551</v>
       </c>
-      <c r="H60" t="s">
-        <v>77</v>
-      </c>
-      <c r="I60" t="s">
-        <v>181</v>
-      </c>
       <c r="J60" t="s">
-        <v>182</v>
+        <v>81</v>
+      </c>
+      <c r="K60" t="s">
+        <v>237</v>
+      </c>
+      <c r="L60" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
         <v>62</v>
@@ -3781,24 +4321,30 @@
         <v>0.822311289245157</v>
       </c>
       <c r="F61" t="s">
-        <v>76</v>
-      </c>
-      <c r="G61" t="n">
+        <v>78</v>
+      </c>
+      <c r="G61" t="s">
+        <v>79</v>
+      </c>
+      <c r="H61" t="s">
+        <v>240</v>
+      </c>
+      <c r="I61" t="n">
         <v>0.284896323258762</v>
       </c>
-      <c r="H61" t="s">
-        <v>82</v>
-      </c>
-      <c r="I61" t="s">
-        <v>181</v>
-      </c>
       <c r="J61" t="s">
-        <v>183</v>
+        <v>87</v>
+      </c>
+      <c r="K61" t="s">
+        <v>237</v>
+      </c>
+      <c r="L61" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
         <v>48</v>
@@ -3813,24 +4359,30 @@
         <v>0.679487179487179</v>
       </c>
       <c r="F62" t="s">
-        <v>112</v>
-      </c>
-      <c r="G62" t="n">
+        <v>136</v>
+      </c>
+      <c r="G62" t="s">
+        <v>99</v>
+      </c>
+      <c r="H62" t="s">
+        <v>231</v>
+      </c>
+      <c r="I62" t="n">
         <v>0.198426573426573</v>
       </c>
-      <c r="H62" t="s">
-        <v>77</v>
-      </c>
-      <c r="I62" t="s">
-        <v>181</v>
-      </c>
       <c r="J62" t="s">
-        <v>184</v>
+        <v>81</v>
+      </c>
+      <c r="K62" t="s">
+        <v>237</v>
+      </c>
+      <c r="L62" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B63" t="s">
         <v>27</v>
@@ -3845,56 +4397,68 @@
         <v>0.247946611909651</v>
       </c>
       <c r="F63" t="s">
-        <v>76</v>
-      </c>
-      <c r="G63" t="n">
+        <v>78</v>
+      </c>
+      <c r="G63" t="s">
+        <v>79</v>
+      </c>
+      <c r="H63" t="s">
+        <v>80</v>
+      </c>
+      <c r="I63" t="n">
         <v>0.218720054757016</v>
       </c>
-      <c r="H63" t="s">
-        <v>77</v>
-      </c>
-      <c r="I63" t="s">
-        <v>181</v>
-      </c>
       <c r="J63" t="s">
-        <v>184</v>
+        <v>81</v>
+      </c>
+      <c r="K63" t="s">
+        <v>237</v>
+      </c>
+      <c r="L63" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="C64" t="n">
         <v>0.503703703703704</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>244</v>
       </c>
       <c r="E64" t="n">
         <v>0.737373737373737</v>
       </c>
       <c r="F64" t="s">
-        <v>131</v>
-      </c>
-      <c r="G64" t="n">
+        <v>163</v>
+      </c>
+      <c r="G64" t="s">
+        <v>79</v>
+      </c>
+      <c r="H64" t="s">
+        <v>245</v>
+      </c>
+      <c r="I64" t="n">
         <v>0.233670033670034</v>
       </c>
-      <c r="H64" t="s">
-        <v>77</v>
-      </c>
-      <c r="I64" t="s">
-        <v>181</v>
-      </c>
       <c r="J64" t="s">
-        <v>187</v>
+        <v>81</v>
+      </c>
+      <c r="K64" t="s">
+        <v>237</v>
+      </c>
+      <c r="L64" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
         <v>58</v>
@@ -3909,51 +4473,63 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
+        <v>107</v>
+      </c>
+      <c r="G65" t="s">
         <v>91</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="s">
+        <v>209</v>
+      </c>
+      <c r="I65" t="n">
         <v>0.471544715447154</v>
       </c>
-      <c r="H65" t="s">
-        <v>82</v>
-      </c>
-      <c r="I65" t="s">
-        <v>181</v>
-      </c>
       <c r="J65" t="s">
-        <v>188</v>
+        <v>87</v>
+      </c>
+      <c r="K65" t="s">
+        <v>237</v>
+      </c>
+      <c r="L65" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
       <c r="C66" t="n">
         <v>0.377777777777778</v>
       </c>
       <c r="D66" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="E66" t="n">
         <v>0.640247859519005</v>
       </c>
       <c r="F66" t="s">
-        <v>94</v>
-      </c>
-      <c r="G66" t="n">
+        <v>112</v>
+      </c>
+      <c r="G66" t="s">
+        <v>91</v>
+      </c>
+      <c r="H66" t="s">
+        <v>250</v>
+      </c>
+      <c r="I66" t="n">
         <v>0.262470081741228</v>
       </c>
-      <c r="H66" t="s">
-        <v>82</v>
-      </c>
-      <c r="I66" t="s">
-        <v>181</v>
-      </c>
       <c r="J66" t="s">
-        <v>191</v>
+        <v>87</v>
+      </c>
+      <c r="K66" t="s">
+        <v>237</v>
+      </c>
+      <c r="L66" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3972,19 +4548,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>252</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>253</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>255</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>256</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -3995,7 +4571,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>257</v>
       </c>
       <c r="C2" t="n">
         <v>0.510666666666667</v>
@@ -4015,7 +4591,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>258</v>
       </c>
       <c r="C3" t="n">
         <v>0.489333333333333</v>
@@ -4035,7 +4611,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="C4" t="n">
         <v>0.0766666666666667</v>
@@ -4055,7 +4631,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="C5" t="n">
         <v>0.155333333333333</v>
@@ -4075,7 +4651,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="C6" t="n">
         <v>0.193333333333333</v>
@@ -4095,7 +4671,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="C7" t="n">
         <v>0.181666666666667</v>
@@ -4115,7 +4691,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
       <c r="C8" t="n">
         <v>0.146666666666667</v>
@@ -4135,7 +4711,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>204</v>
+        <v>264</v>
       </c>
       <c r="C9" t="n">
         <v>0.246666666666667</v>

</xml_diff>